<commit_message>
5 apr - out of service debuging
</commit_message>
<xml_diff>
--- a/12附着反力计算compare.xlsx
+++ b/12附着反力计算compare.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12360" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12360" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="（工作状态）-80116(high)100m以上" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
@@ -60,14 +61,19 @@
     <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
@@ -85,6 +91,7 @@
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.001</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
@@ -126,7 +133,9 @@
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
@@ -136,6 +145,7 @@
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">100</definedName>
@@ -153,6 +163,7 @@
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1740,6 +1751,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1756,12 +1773,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3527,17 +3538,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="60" customHeight="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:18" ht="60" customHeight="1"/>
     <row r="3" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -3752,15 +3763,15 @@
       <c r="F16" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="46" t="s">
+      <c r="L16" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
     </row>
     <row r="17" spans="1:21" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B17" t="s">
@@ -3776,7 +3787,7 @@
       <c r="F17" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="46" t="s">
+      <c r="L17" s="48" t="s">
         <v>70</v>
       </c>
       <c r="M17">
@@ -3792,7 +3803,7 @@
     <row r="18" spans="1:21" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="D18" s="6"/>
       <c r="E18" s="15"/>
-      <c r="L18" s="46"/>
+      <c r="L18" s="48"/>
       <c r="M18">
         <f t="shared" si="0"/>
         <v>259.5</v>
@@ -3806,7 +3817,7 @@
     <row r="19" spans="1:21" ht="20.100000000000001" customHeight="1">
       <c r="D19" s="6"/>
       <c r="E19" s="15"/>
-      <c r="L19" s="46"/>
+      <c r="L19" s="48"/>
       <c r="M19">
         <f t="shared" si="0"/>
         <v>219.60000000000002</v>
@@ -3821,7 +3832,7 @@
       <c r="U19" s="39"/>
     </row>
     <row r="20" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="L20" s="46"/>
+      <c r="L20" s="48"/>
       <c r="M20">
         <f t="shared" si="0"/>
         <v>179.70000000000002</v>
@@ -3843,7 +3854,7 @@
       <c r="H21" t="s">
         <v>58</v>
       </c>
-      <c r="L21" s="46"/>
+      <c r="L21" s="48"/>
       <c r="M21">
         <f t="shared" si="0"/>
         <v>139.80000000000001</v>
@@ -3886,7 +3897,7 @@
         <f>F22*20</f>
         <v>22484.210526315786</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="48"/>
       <c r="M22">
         <f>M23+39.9</f>
         <v>99.9</v>
@@ -3929,7 +3940,7 @@
         <f>F23*80</f>
         <v>89936.842105263146</v>
       </c>
-      <c r="L23" s="46"/>
+      <c r="L23" s="48"/>
       <c r="M23">
         <v>60</v>
       </c>
@@ -3976,10 +3987,10 @@
         <f>F24*(E17-B6)</f>
         <v>47947.57894736842</v>
       </c>
-      <c r="L24" s="46" t="s">
+      <c r="L24" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="M24" s="46"/>
+      <c r="M24" s="48"/>
       <c r="N24">
         <v>18</v>
       </c>
@@ -4049,10 +4060,10 @@
         <v>31</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="L26" s="46" t="s">
+      <c r="L26" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="M26" s="46"/>
+      <c r="M26" s="48"/>
       <c r="S26" s="39"/>
       <c r="T26" s="39"/>
       <c r="U26" s="39"/>
@@ -4080,10 +4091,10 @@
       <c r="I27" s="20">
         <v>6</v>
       </c>
-      <c r="L27" s="46" t="s">
+      <c r="L27" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="M27" s="46"/>
+      <c r="M27" s="48"/>
       <c r="N27">
         <v>49.58</v>
       </c>
@@ -4130,10 +4141,10 @@
       <c r="I28" s="19">
         <v>0</v>
       </c>
-      <c r="L28" s="46" t="s">
+      <c r="L28" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="M28" s="46"/>
+      <c r="M28" s="48"/>
       <c r="N28">
         <v>-720.32</v>
       </c>
@@ -4320,10 +4331,10 @@
       <c r="L33" s="26"/>
     </row>
     <row r="34" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="48"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="22">
         <f>IF($E$13=0,0,IF(D28&lt;$E$13,10^4*$E$12*$E$13^3/3*(1-3*($E$13-D28)/(2*$E$13)+($E$13-D28)^3/(2*$E$13^3)),10^4*$E$12*$E$13^3/3*(1+3*(D28-$E$13)/(2*$E$13))))</f>
         <v>0</v>
@@ -4352,10 +4363,10 @@
       <c r="L34" s="26"/>
     </row>
     <row r="35" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="50"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="22">
         <f>SUM(D29:D34)</f>
         <v>17430098303.74358</v>
@@ -4436,10 +4447,10 @@
       </c>
     </row>
     <row r="38" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="51"/>
+      <c r="C38" s="53"/>
       <c r="D38" s="7">
         <v>1</v>
       </c>
@@ -4837,10 +4848,10 @@
       </c>
     </row>
     <row r="59" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="M59" s="46" t="s">
+      <c r="M59" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="N59" s="46"/>
+      <c r="N59" s="48"/>
       <c r="O59">
         <v>252.38</v>
       </c>
@@ -5871,17 +5882,17 @@
     </scenario>
   </scenarios>
   <mergeCells count="11">
+    <mergeCell ref="M59:N59"/>
+    <mergeCell ref="L16:R16"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="L28:M28"/>
     <mergeCell ref="L17:L23"/>
     <mergeCell ref="L24:M24"/>
     <mergeCell ref="L26:M26"/>
     <mergeCell ref="L27:M27"/>
-    <mergeCell ref="M59:N59"/>
-    <mergeCell ref="L16:R16"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B38:C38"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5920,17 +5931,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="60" customHeight="1">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="60" customHeight="1"/>
     <row r="3" spans="1:21" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -6017,18 +6028,18 @@
       <c r="G6" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="46" t="s">
+      <c r="L6" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
     </row>
     <row r="7" spans="1:21" ht="20.100000000000001" customHeight="1" thickTop="1">
-      <c r="L7" s="46" t="s">
+      <c r="L7" s="48" t="s">
         <v>70</v>
       </c>
       <c r="M7">
@@ -6045,7 +6056,7 @@
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="46"/>
+      <c r="L8" s="48"/>
       <c r="M8">
         <f t="shared" si="0"/>
         <v>259.5</v>
@@ -6069,7 +6080,7 @@
       <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="46"/>
+      <c r="L9" s="48"/>
       <c r="M9">
         <f t="shared" si="0"/>
         <v>219.60000000000002</v>
@@ -6096,7 +6107,7 @@
       <c r="F10" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="46"/>
+      <c r="L10" s="48"/>
       <c r="M10">
         <f t="shared" si="0"/>
         <v>179.70000000000002</v>
@@ -6124,7 +6135,7 @@
       <c r="F11" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="46"/>
+      <c r="L11" s="48"/>
       <c r="M11">
         <f t="shared" si="0"/>
         <v>139.80000000000001</v>
@@ -6154,7 +6165,7 @@
       <c r="F12" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="46"/>
+      <c r="L12" s="48"/>
       <c r="M12">
         <f>M13+39.9</f>
         <v>99.9</v>
@@ -6184,7 +6195,7 @@
       <c r="F13" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="46"/>
+      <c r="L13" s="48"/>
       <c r="M13">
         <v>60</v>
       </c>
@@ -6219,10 +6230,10 @@
       <c r="F14" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="46" t="s">
+      <c r="L14" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="M14" s="46"/>
+      <c r="M14" s="48"/>
       <c r="N14">
         <v>18</v>
       </c>
@@ -6309,10 +6320,10 @@
       <c r="F16" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="46" t="s">
+      <c r="L16" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="M16" s="46"/>
+      <c r="M16" s="48"/>
       <c r="S16" s="39"/>
       <c r="T16" s="39"/>
       <c r="U16" s="39"/>
@@ -6331,10 +6342,10 @@
       <c r="F17" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="46" t="s">
+      <c r="L17" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="M17" s="46"/>
+      <c r="M17" s="48"/>
       <c r="N17">
         <v>74.81</v>
       </c>
@@ -6361,10 +6372,10 @@
     <row r="18" spans="1:21" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="D18" s="6"/>
       <c r="E18" s="15"/>
-      <c r="L18" s="46" t="s">
+      <c r="L18" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="M18" s="46"/>
+      <c r="M18" s="48"/>
       <c r="N18">
         <v>-298.27999999999997</v>
       </c>
@@ -6702,10 +6713,10 @@
       <c r="L33" s="26"/>
     </row>
     <row r="34" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="48"/>
+      <c r="C34" s="50"/>
       <c r="D34" s="22">
         <f>IF($E$13=0,0,IF(D28&lt;$E$13,10^4*$E$12*$E$13^3/3*(1-3*($E$13-D28)/(2*$E$13)+($E$13-D28)^3/(2*$E$13^3)),10^4*$E$12*$E$13^3/3*(1+3*(D28-$E$13)/(2*$E$13))))</f>
         <v>0</v>
@@ -6734,10 +6745,10 @@
       <c r="L34" s="26"/>
     </row>
     <row r="35" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="50"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="22">
         <f>SUM(D29:D34)</f>
         <v>39119982215.989388</v>
@@ -6808,10 +6819,10 @@
       <c r="O37" s="30"/>
     </row>
     <row r="38" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="51"/>
+      <c r="C38" s="53"/>
       <c r="D38" s="7">
         <v>1</v>
       </c>
@@ -7186,10 +7197,10 @@
       <c r="G55" s="34"/>
       <c r="H55" s="34"/>
       <c r="I55" s="34"/>
-      <c r="L55" s="46" t="s">
+      <c r="L55" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="M55" s="46"/>
+      <c r="M55" s="48"/>
       <c r="N55">
         <v>263.04000000000002</v>
       </c>
@@ -7243,8 +7254,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -7714,10 +7725,10 @@
       <c r="L30" s="26"/>
     </row>
     <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1" outlineLevel="1">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="48"/>
+      <c r="C31" s="50"/>
       <c r="D31" s="22">
         <f>IF($E$12=0,0,IF(D26&lt;$E$12,10^4*$E$11*$E$12^3/3*(1-3*($E$12-D26)/(2*$E$12)+($E$12-D26)^3/(2*$E$12^3)),10^4*$E$11*$E$12^3/3*(1+3*(D26-$E$12)/(2*$E$12))))</f>
         <v>0</v>
@@ -7746,10 +7757,10 @@
       <c r="L31" s="26"/>
     </row>
     <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1" outlineLevel="1">
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="50"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="22">
         <f>SUM(D27:D31)</f>
         <v>1929410156.52</v>
@@ -7829,10 +7840,10 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1" outlineLevel="1">
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="51"/>
+      <c r="C35" s="53"/>
       <c r="D35" s="7">
         <v>1</v>
       </c>
@@ -8073,11 +8084,11 @@
       </c>
       <c r="D44" s="22">
         <f>$D$50*D36+$E$50*D37+$F$50*D38+$G$50*D39+$H$50*D40+$I$50*D41-D32</f>
-        <v>-905516888.66470671</v>
+        <v>4275911849.9758811</v>
       </c>
       <c r="E44" s="22">
         <f t="shared" ref="E44:I44" si="13">$D$50*E36+$E$50*E37+$F$50*E38+$G$50*E39+$H$50*E40+$I$50*E41-E32</f>
-        <v>-2006570702.7423534</v>
+        <v>7482845737.4577694</v>
       </c>
       <c r="F44" s="22">
         <f t="shared" si="13"/>
@@ -8102,11 +8113,11 @@
       </c>
       <c r="D45" s="22">
         <f>D44/$D$46</f>
-        <v>-9055.1688866470668</v>
+        <v>42759.118499758813</v>
       </c>
       <c r="E45" s="22">
         <f t="shared" ref="E45:H45" si="14">E44/$D$46</f>
-        <v>-20065.707027423534</v>
+        <v>74828.457374577687</v>
       </c>
       <c r="F45" s="22">
         <f t="shared" si="14"/>
@@ -8169,10 +8180,10 @@
         <v>63</v>
       </c>
       <c r="D50" s="32">
-        <v>-337827.97311580979</v>
+        <v>273868.70921875024</v>
       </c>
       <c r="E50" s="32">
-        <v>320015.44741727988</v>
+        <v>613012.77212498512</v>
       </c>
       <c r="F50" s="32">
         <v>628931.40473403619</v>
@@ -8201,7 +8212,7 @@
       <c r="D53" s="7"/>
       <c r="E53" s="37">
         <f>(($B$5-0)^2*$F$21/2+(E16-$B$5)*$F$22*(E16+$B$5)/2)/10^4+E8+$E$9*$E$10+$E$11*$E$12-(D50*D26+E50*E26+F50*F26+G50*G26+H50*H26+I50*I26)/10^4</f>
-        <v>357.65756690073601</v>
+        <v>-2165.2048396499467</v>
       </c>
     </row>
   </sheetData>
@@ -8226,8 +8237,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -8343,7 +8354,7 @@
       </c>
       <c r="E10" s="5">
         <f>E16+3</f>
-        <v>60.15</v>
+        <v>45.15</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -8399,7 +8410,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="5">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
@@ -8429,7 +8440,7 @@
       </c>
       <c r="E16" s="5">
         <f>E13*E14+0.15</f>
-        <v>57.15</v>
+        <v>42.15</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -8503,13 +8514,13 @@
       </c>
       <c r="H22">
         <f>F22*(E16-B22)</f>
-        <v>83854.98</v>
+        <v>49996.979999999996</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="H23">
         <f>SUM(H21:H22)+E9*10000</f>
-        <v>136686.97999999998</v>
+        <v>102828.98</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="20.100000000000001" customHeight="1">
@@ -8551,7 +8562,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="19">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="F26" s="19">
         <v>0</v>
@@ -8577,7 +8588,7 @@
       </c>
       <c r="E27" s="22">
         <f t="shared" si="0"/>
-        <v>67852800</v>
+        <v>0</v>
       </c>
       <c r="F27" s="22">
         <f t="shared" si="0"/>
@@ -8605,11 +8616,11 @@
       <c r="C28" s="14"/>
       <c r="D28" s="22">
         <f>IF(D26&lt;$B$5,$F$22*($E$16-$B$5)/12*(3*($E$16+$B$5)*D26^2-2*D26^3),$F$22*($E$16-$B$5)/24*(6*($E$16+$B$5)*D26^2-4*D26^3+(D26-$B$5)^4/($E$16-$B$5)))</f>
-        <v>738417488.68800008</v>
+        <v>332284007.088</v>
       </c>
       <c r="E28" s="22">
         <f t="shared" ref="E28:I28" si="1">IF(E26&lt;$B$5,$F$22*($E$16-$B$5)/12*(3*($E$16+$B$5)*E26^2-2*E26^3),$F$22*($E$16-$B$5)/24*(6*($E$16+$B$5)*E26^2-4*E26^3+(E26-$B$5)^4/($E$16-$B$5)))</f>
-        <v>1450196729.388</v>
+        <v>0</v>
       </c>
       <c r="F28" s="22">
         <f t="shared" si="1"/>
@@ -8641,7 +8652,7 @@
       </c>
       <c r="E29" s="22">
         <f t="shared" ref="E29:I29" si="2">$E$8*10^4/2*E26^2</f>
-        <v>3596400000</v>
+        <v>0</v>
       </c>
       <c r="F29" s="22">
         <f t="shared" si="2"/>
@@ -8669,11 +8680,11 @@
       <c r="C30" s="14"/>
       <c r="D30" s="22">
         <f>IF($E$9=0,0,10^4*$E$9*$E$10^3/3*(1-3*($E$10-D26)/(2*$E$10)+($E$10-D26)^3/(2*$E$10^3)))</f>
-        <v>300384000.00000006</v>
+        <v>213983999.99999994</v>
       </c>
       <c r="E30" s="22">
         <f t="shared" ref="E30:I30" si="3">IF($E$9=0,0,10^4*$E$9*$E$10^3/3*(1-3*($E$10-E26)/(2*$E$10)+($E$10-E26)^3/(2*$E$10^3)))</f>
-        <v>624024000.00000012</v>
+        <v>0</v>
       </c>
       <c r="F30" s="22">
         <f t="shared" si="3"/>
@@ -8695,10 +8706,10 @@
       <c r="L30" s="26"/>
     </row>
     <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1" outlineLevel="1">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="48"/>
+      <c r="C31" s="50"/>
       <c r="D31" s="22">
         <f>IF($E$12=0,0,IF(D26&lt;$E$12,10^4*$E$11*$E$12^3/3*(1-3*($E$12-D26)/(2*$E$12)+($E$12-D26)^3/(2*$E$12^3)),10^4*$E$11*$E$12^3/3*(1+3*(D26-$E$12)/(2*$E$12))))</f>
         <v>0</v>
@@ -8727,17 +8738,17 @@
       <c r="L31" s="26"/>
     </row>
     <row r="32" spans="1:13" ht="20.100000000000001" customHeight="1" outlineLevel="1">
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="50"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="22">
         <f>SUM(D27:D31)</f>
-        <v>2678788688.6880002</v>
+        <v>2186255207.0879998</v>
       </c>
       <c r="E32" s="22">
         <f>SUM(E27:E31)</f>
-        <v>5738473529.3880005</v>
+        <v>0</v>
       </c>
       <c r="F32" s="22">
         <f t="shared" ref="F32:I32" si="5">SUM(F27:F31)</f>
@@ -8765,11 +8776,11 @@
       </c>
       <c r="D33" s="29">
         <f>D32/$O$34</f>
-        <v>0.19314519478697276</v>
+        <v>0.15763269779739858</v>
       </c>
       <c r="E33" s="29">
         <f t="shared" ref="E33:I33" si="6">E32/$O$34</f>
-        <v>0.41375364630062594</v>
+        <v>0</v>
       </c>
       <c r="F33" s="29">
         <f t="shared" si="6"/>
@@ -8810,10 +8821,10 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="20.100000000000001" customHeight="1" outlineLevel="1">
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="51"/>
+      <c r="C35" s="53"/>
       <c r="D35" s="7">
         <v>1</v>
       </c>
@@ -8849,7 +8860,7 @@
       </c>
       <c r="E36" s="23">
         <f t="shared" ref="E36:I36" si="7">IF($D$26=0,0,IF(E26&lt;$D$26,1*$D$26^3/3*(1-3*($D$26-E26)/2/$D$26+($D$26-E26)^3/2/$D$26^3),1*$D$26^3/3*(1+3*(E26-$D$26)/2/$D$26)))</f>
-        <v>8064</v>
+        <v>0</v>
       </c>
       <c r="F36" s="23">
         <f t="shared" si="7"/>
@@ -8873,7 +8884,7 @@
       </c>
       <c r="N36" s="31">
         <f>E36/$O$34</f>
-        <v>5.8142803773185331E-7</v>
+        <v>0</v>
       </c>
       <c r="O36" s="38"/>
     </row>
@@ -8886,11 +8897,11 @@
       </c>
       <c r="D37" s="23">
         <f>IF($E$26=0,0,IF(D26&lt;$E$26,1*$E$26^3/3*(1-3*($E$26-D26)/2/$E$26+($E$26-D26)^3/2/$E$26^3),1*$E$26^3/3*(1+3*(D26-$E$26)/2/$E$26)))</f>
-        <v>8064</v>
+        <v>0</v>
       </c>
       <c r="E37" s="23">
         <f t="shared" ref="E37:I37" si="8">IF($E$26=0,0,IF(E26&lt;$E$26,1*$E$26^3/3*(1-3*($E$26-E26)/2/$E$26+($E$26-E26)^3/2/$E$26^3),1*$E$26^3/3*(1+3*(E26-$E$26)/2/$E$26)))</f>
-        <v>15552</v>
+        <v>0</v>
       </c>
       <c r="F37" s="23">
         <f t="shared" si="8"/>
@@ -8910,11 +8921,11 @@
       </c>
       <c r="M37" s="31">
         <f>D37/$O$34</f>
-        <v>5.8142803773185331E-7</v>
+        <v>0</v>
       </c>
       <c r="N37" s="31">
         <f>E37/$O$34</f>
-        <v>1.1213255013400027E-6</v>
+        <v>0</v>
       </c>
       <c r="O37" s="38"/>
     </row>
@@ -9054,11 +9065,11 @@
       </c>
       <c r="D44" s="22">
         <f>$D$50*D36+$E$50*D37+$F$50*D38+$G$50*D39+$H$50*D40+$I$50*D41-D32</f>
-        <v>931969792.20344877</v>
+        <v>0</v>
       </c>
       <c r="E44" s="22">
         <f t="shared" ref="E44:I44" si="13">$D$50*E36+$E$50*E37+$F$50*E38+$G$50*E39+$H$50*E40+$I$50*E41-E32</f>
-        <v>1116630950.3420219</v>
+        <v>0</v>
       </c>
       <c r="F44" s="22">
         <f t="shared" si="13"/>
@@ -9083,11 +9094,11 @@
       </c>
       <c r="D45" s="22">
         <f>D44/$D$46</f>
-        <v>9319.6979220344874</v>
+        <v>0</v>
       </c>
       <c r="E45" s="22">
         <f t="shared" ref="E45:I45" si="14">E44/$D$46</f>
-        <v>11166.30950342022</v>
+        <v>0</v>
       </c>
       <c r="F45" s="22">
         <f t="shared" si="14"/>
@@ -9150,10 +9161,10 @@
         <v>63</v>
       </c>
       <c r="D50" s="32">
-        <v>131859.05102854338</v>
+        <v>474447.74459375028</v>
       </c>
       <c r="E50" s="32">
-        <v>372414.67928471247</v>
+        <v>729578.69734998746</v>
       </c>
       <c r="F50" s="32">
         <v>0</v>
@@ -9182,7 +9193,7 @@
       <c r="D53" s="7"/>
       <c r="E53" s="37">
         <f>(($B$5-0)^2*$F$21/2+(E16-$B$5)*$F$22*(E16+$B$5)/2)/10^4+E8+$E$9*$E$10+$E$11*$E$12-(D50*D26+E50*E26+F50*F26+G50*G26+H50*H26+I50*I26)/10^4</f>
-        <v>-625.55198254346897</v>
+        <v>-305.17697167500069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
13 July sympy in service ok, check out of service, different wind pressure with height position
</commit_message>
<xml_diff>
--- a/12附着反力计算compare.xlsx
+++ b/12附着反力计算compare.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA762E32-35C4-4CA8-975C-62C2D6BE852E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12360" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="（工作状态）-80116(high)100m以上" sheetId="1" r:id="rId1"/>
@@ -165,17 +166,25 @@
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F15" authorId="0" shapeId="0">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -220,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -274,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -309,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="0" shapeId="0">
+    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -354,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M23" authorId="0" shapeId="0">
+    <comment ref="M23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -404,12 +413,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="M12" authorId="0" shapeId="0">
+    <comment ref="M12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -454,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M13" authorId="0" shapeId="0">
+    <comment ref="M13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -499,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -544,7 +553,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -598,7 +607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -638,12 +647,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F14" authorId="0" shapeId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -688,7 +697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -742,7 +751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -782,12 +791,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F14" authorId="0" shapeId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -832,7 +841,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -886,7 +895,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1307,7 +1316,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
@@ -1816,7 +1825,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -1880,7 +1895,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -1944,7 +1965,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2008,7 +2035,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2072,7 +2105,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2136,7 +2175,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2205,7 +2250,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2269,7 +2320,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2333,7 +2390,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2397,7 +2460,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2461,7 +2530,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2525,7 +2600,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2594,7 +2675,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks/>
         </xdr:cNvSpPr>
@@ -2658,7 +2745,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2722,7 +2815,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -2786,7 +2885,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks/>
         </xdr:cNvSpPr>
@@ -2850,7 +2955,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="TextBox 8"/>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks/>
         </xdr:cNvSpPr>
@@ -2919,7 +3030,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks/>
         </xdr:cNvSpPr>
@@ -2983,7 +3100,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -3047,7 +3170,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
@@ -3111,7 +3240,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks/>
         </xdr:cNvSpPr>
@@ -3175,7 +3310,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks/>
         </xdr:cNvSpPr>
@@ -3303,6 +3444,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3338,6 +3496,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3513,7 +3688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -5906,7 +6081,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -7248,14 +7423,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -8084,11 +8259,11 @@
       </c>
       <c r="D44" s="22">
         <f>$D$50*D36+$E$50*D37+$F$50*D38+$G$50*D39+$H$50*D40+$I$50*D41-D32</f>
-        <v>4275911849.9758811</v>
+        <v>-84.975912570953369</v>
       </c>
       <c r="E44" s="22">
         <f t="shared" ref="E44:I44" si="13">$D$50*E36+$E$50*E37+$F$50*E38+$G$50*E39+$H$50*E40+$I$50*E41-E32</f>
-        <v>7482845737.4577694</v>
+        <v>-99.999999523162842</v>
       </c>
       <c r="F44" s="22">
         <f t="shared" si="13"/>
@@ -8113,11 +8288,11 @@
       </c>
       <c r="D45" s="22">
         <f>D44/$D$46</f>
-        <v>42759.118499758813</v>
+        <v>-8.4975912570953366E-4</v>
       </c>
       <c r="E45" s="22">
         <f t="shared" ref="E45:H45" si="14">E44/$D$46</f>
-        <v>74828.457374577687</v>
+        <v>-9.9999999523162834E-4</v>
       </c>
       <c r="F45" s="22">
         <f t="shared" si="14"/>
@@ -8180,10 +8355,10 @@
         <v>63</v>
       </c>
       <c r="D50" s="32">
-        <v>273868.70921875024</v>
+        <v>-654063.62752514088</v>
       </c>
       <c r="E50" s="32">
-        <v>613012.77212498512</v>
+        <v>613012.80594989297</v>
       </c>
       <c r="F50" s="32">
         <v>628931.40473403619</v>
@@ -8212,7 +8387,7 @@
       <c r="D53" s="7"/>
       <c r="E53" s="37">
         <f>(($B$5-0)^2*$F$21/2+(E16-$B$5)*$F$22*(E16+$B$5)/2)/10^4+E8+$E$9*$E$10+$E$11*$E$12-(D50*D26+E50*E26+F50*F26+G50*G26+H50*H26+I50*I26)/10^4</f>
-        <v>-2165.2048396499467</v>
+        <v>61.832646765723325</v>
       </c>
     </row>
   </sheetData>
@@ -8231,14 +8406,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -8353,8 +8528,8 @@
         <v>38</v>
       </c>
       <c r="E10" s="5">
-        <f>E16+3</f>
-        <v>45.15</v>
+        <f>E16</f>
+        <v>72.150000000000006</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
@@ -8410,7 +8585,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="5">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
@@ -8440,7 +8615,7 @@
       </c>
       <c r="E16" s="5">
         <f>E13*E14+0.15</f>
-        <v>42.15</v>
+        <v>72.150000000000006</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -8514,13 +8689,13 @@
       </c>
       <c r="H22">
         <f>F22*(E16-B22)</f>
-        <v>49996.979999999996</v>
+        <v>117712.98000000001</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="H23">
         <f>SUM(H21:H22)+E9*10000</f>
-        <v>102828.98</v>
+        <v>170544.98</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="20.100000000000001" customHeight="1">
@@ -8562,10 +8737,10 @@
         <v>24</v>
       </c>
       <c r="E26" s="19">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="F26" s="19">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="G26" s="19">
         <v>0</v>
@@ -8588,11 +8763,11 @@
       </c>
       <c r="E27" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67852800</v>
       </c>
       <c r="F27" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>94118400</v>
       </c>
       <c r="G27" s="22">
         <f t="shared" si="0"/>
@@ -8616,15 +8791,15 @@
       <c r="C28" s="14"/>
       <c r="D28" s="22">
         <f>IF(D26&lt;$B$5,$F$22*($E$16-$B$5)/12*(3*($E$16+$B$5)*D26^2-2*D26^3),$F$22*($E$16-$B$5)/24*(6*($E$16+$B$5)*D26^2-4*D26^3+(D26-$B$5)^4/($E$16-$B$5)))</f>
-        <v>332284007.088</v>
+        <v>1290817530.2880003</v>
       </c>
       <c r="E28" s="22">
         <f t="shared" ref="E28:I28" si="1">IF(E26&lt;$B$5,$F$22*($E$16-$B$5)/12*(3*($E$16+$B$5)*E26^2-2*E26^3),$F$22*($E$16-$B$5)/24*(6*($E$16+$B$5)*E26^2-4*E26^3+(E26-$B$5)^4/($E$16-$B$5)))</f>
-        <v>0</v>
+        <v>2605336886.9880009</v>
       </c>
       <c r="F28" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4136139387.072001</v>
       </c>
       <c r="G28" s="22">
         <f t="shared" si="1"/>
@@ -8652,11 +8827,11 @@
       </c>
       <c r="E29" s="22">
         <f t="shared" ref="E29:I29" si="2">$E$8*10^4/2*E26^2</f>
-        <v>0</v>
+        <v>3596400000</v>
       </c>
       <c r="F29" s="22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6393600000</v>
       </c>
       <c r="G29" s="22">
         <f t="shared" si="2"/>
@@ -8680,15 +8855,15 @@
       <c r="C30" s="14"/>
       <c r="D30" s="22">
         <f>IF($E$9=0,0,10^4*$E$9*$E$10^3/3*(1-3*($E$10-D26)/(2*$E$10)+($E$10-D26)^3/(2*$E$10^3)))</f>
-        <v>213983999.99999994</v>
+        <v>369504000.00000024</v>
       </c>
       <c r="E30" s="22">
         <f t="shared" ref="E30:I30" si="3">IF($E$9=0,0,10^4*$E$9*$E$10^3/3*(1-3*($E$10-E26)/(2*$E$10)+($E$10-E26)^3/(2*$E$10^3)))</f>
-        <v>0</v>
+        <v>779544000</v>
       </c>
       <c r="F30" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1293696000</v>
       </c>
       <c r="G30" s="22">
         <f t="shared" si="3"/>
@@ -8744,15 +8919,15 @@
       <c r="C32" s="52"/>
       <c r="D32" s="22">
         <f>SUM(D27:D31)</f>
-        <v>2186255207.0879998</v>
+        <v>3300308730.2880001</v>
       </c>
       <c r="E32" s="22">
         <f>SUM(E27:E31)</f>
-        <v>0</v>
+        <v>7049133686.9880009</v>
       </c>
       <c r="F32" s="22">
         <f t="shared" ref="F32:I32" si="5">SUM(F27:F31)</f>
-        <v>0</v>
+        <v>11917553787.072001</v>
       </c>
       <c r="G32" s="22">
         <f t="shared" si="5"/>
@@ -8776,15 +8951,15 @@
       </c>
       <c r="D33" s="29">
         <f>D32/$O$34</f>
-        <v>0.15763269779739858</v>
+        <v>0.2379578408929385</v>
       </c>
       <c r="E33" s="29">
         <f t="shared" ref="E33:I33" si="6">E32/$O$34</f>
-        <v>0</v>
+        <v>0.50825446023498722</v>
       </c>
       <c r="F33" s="29">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.85927578285975814</v>
       </c>
       <c r="G33" s="29">
         <f t="shared" si="6"/>
@@ -8860,11 +9035,11 @@
       </c>
       <c r="E36" s="23">
         <f t="shared" ref="E36:I36" si="7">IF($D$26=0,0,IF(E26&lt;$D$26,1*$D$26^3/3*(1-3*($D$26-E26)/2/$D$26+($D$26-E26)^3/2/$D$26^3),1*$D$26^3/3*(1+3*(E26-$D$26)/2/$D$26)))</f>
-        <v>0</v>
+        <v>8064</v>
       </c>
       <c r="F36" s="23">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>11520</v>
       </c>
       <c r="G36" s="23">
         <f t="shared" si="7"/>
@@ -8884,7 +9059,7 @@
       </c>
       <c r="N36" s="31">
         <f>E36/$O$34</f>
-        <v>0</v>
+        <v>5.8142803773185331E-7</v>
       </c>
       <c r="O36" s="38"/>
     </row>
@@ -8897,15 +9072,15 @@
       </c>
       <c r="D37" s="23">
         <f>IF($E$26=0,0,IF(D26&lt;$E$26,1*$E$26^3/3*(1-3*($E$26-D26)/2/$E$26+($E$26-D26)^3/2/$E$26^3),1*$E$26^3/3*(1+3*(D26-$E$26)/2/$E$26)))</f>
-        <v>0</v>
+        <v>8064</v>
       </c>
       <c r="E37" s="23">
         <f t="shared" ref="E37:I37" si="8">IF($E$26=0,0,IF(E26&lt;$E$26,1*$E$26^3/3*(1-3*($E$26-E26)/2/$E$26+($E$26-E26)^3/2/$E$26^3),1*$E$26^3/3*(1+3*(E26-$E$26)/2/$E$26)))</f>
-        <v>0</v>
+        <v>15552</v>
       </c>
       <c r="F37" s="23">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>23328</v>
       </c>
       <c r="G37" s="23">
         <f t="shared" si="8"/>
@@ -8921,11 +9096,11 @@
       </c>
       <c r="M37" s="31">
         <f>D37/$O$34</f>
-        <v>0</v>
+        <v>5.8142803773185331E-7</v>
       </c>
       <c r="N37" s="31">
         <f>E37/$O$34</f>
-        <v>0</v>
+        <v>1.1213255013400027E-6</v>
       </c>
       <c r="O37" s="38"/>
     </row>
@@ -8938,15 +9113,15 @@
       </c>
       <c r="D38" s="23">
         <f>IF($F$26=0,0,IF(D26&lt;$F$26,1*$F$26^3/3*(1-3*($F$26-D26)/2/$F$26+($F$26-D26)^3/2/$F$26^3),1*$F$26^3/3*(1+3*(D26-$F$26)/2/$F$26)))</f>
-        <v>0</v>
+        <v>11520</v>
       </c>
       <c r="E38" s="23">
         <f t="shared" ref="E38:I38" si="9">IF($F$26=0,0,IF(E26&lt;$F$26,1*$F$26^3/3*(1-3*($F$26-E26)/2/$F$26+($F$26-E26)^3/2/$F$26^3),1*$F$26^3/3*(1+3*(E26-$F$26)/2/$F$26)))</f>
-        <v>0</v>
+        <v>23328</v>
       </c>
       <c r="F38" s="23">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>36864</v>
       </c>
       <c r="G38" s="23">
         <f t="shared" si="9"/>
@@ -9065,15 +9240,15 @@
       </c>
       <c r="D44" s="22">
         <f>$D$50*D36+$E$50*D37+$F$50*D38+$G$50*D39+$H$50*D40+$I$50*D41-D32</f>
-        <v>0</v>
+        <v>-222067455.04793072</v>
       </c>
       <c r="E44" s="22">
         <f t="shared" ref="E44:I44" si="13">$D$50*E36+$E$50*E37+$F$50*E38+$G$50*E39+$H$50*E40+$I$50*E41-E32</f>
-        <v>0</v>
+        <v>-445531614.49793434</v>
       </c>
       <c r="F44" s="22">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-705042964.51196861</v>
       </c>
       <c r="G44" s="22">
         <f t="shared" si="13"/>
@@ -9094,15 +9269,15 @@
       </c>
       <c r="D45" s="22">
         <f>D44/$D$46</f>
-        <v>0</v>
+        <v>-2220.6745504793071</v>
       </c>
       <c r="E45" s="22">
         <f t="shared" ref="E45:I45" si="14">E44/$D$46</f>
-        <v>0</v>
+        <v>-4455.3161449793433</v>
       </c>
       <c r="F45" s="22">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-7050.429645119686</v>
       </c>
       <c r="G45" s="22">
         <f t="shared" si="14"/>
@@ -9161,13 +9336,13 @@
         <v>63</v>
       </c>
       <c r="D50" s="32">
-        <v>474447.74459375028</v>
+        <v>225862.84161600206</v>
       </c>
       <c r="E50" s="32">
-        <v>729578.69734998746</v>
+        <v>-844106.07384867023</v>
       </c>
       <c r="F50" s="32">
-        <v>0</v>
+        <v>767737.55907892436</v>
       </c>
       <c r="G50" s="32">
         <v>0</v>
@@ -9193,7 +9368,7 @@
       <c r="D53" s="7"/>
       <c r="E53" s="37">
         <f>(($B$5-0)^2*$F$21/2+(E16-$B$5)*$F$22*(E16+$B$5)/2)/10^4+E8+$E$9*$E$10+$E$11*$E$12-(D50*D26+E50*E26+F50*F26+G50*G26+H50*H26+I50*I26)/10^4</f>
-        <v>-305.17697167500069</v>
+        <v>86.065317747970994</v>
       </c>
     </row>
   </sheetData>
@@ -9212,7 +9387,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>